<commit_message>
02--Formula contract payment advance
</commit_message>
<xml_diff>
--- a/Contract formula.xlsx
+++ b/Contract formula.xlsx
@@ -597,10 +597,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -908,7 +908,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -920,7 +920,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -984,7 +984,7 @@
         <f ca="1">IF(AND(B2="C001", C2&gt;0,E2=0),C2,IF(AND(B2="C001", H2 &gt; 0),J1-(I2+H2),J1-I2))</f>
         <v>10000</v>
       </c>
-      <c r="L2" s="41">
+      <c r="L2" s="40">
         <v>0.1</v>
       </c>
     </row>
@@ -1065,12 +1065,13 @@
         <v>4000</v>
       </c>
       <c r="J5">
-        <f t="shared" ref="J3:J5" ca="1" si="0">IF(AND(B5="C001", C5&gt;0,E5=0),C5,IF(AND(B5="C001", H5 &gt; 0),J4-(I5+H5),J4-I5))</f>
+        <f ca="1">IF(AND(B5="C001", C5&gt;0,E5=0),C5,IF(AND(B5="C001", H5 &gt; 0),J4-(I5+H5),J4-I5))</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1103,17 +1104,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
       <c r="K1" s="22"/>
       <c r="L1" s="22"/>
     </row>

</xml_diff>

<commit_message>
adding print feature to report
</commit_message>
<xml_diff>
--- a/Contract formula.xlsx
+++ b/Contract formula.xlsx
@@ -33,6 +33,64 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Vandert THUY</author>
+  </authors>
+  <commentList>
+    <comment ref="F3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Vandert THUY:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Contract Balance minus Advance amt</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Vandert THUY:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Advance Amt - Contract Balance - 1</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Vandert THUY</author>
@@ -140,7 +198,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
   <si>
     <t>Contract No.</t>
   </si>
@@ -308,6 +366,9 @@
   </si>
   <si>
     <t>If &gt; Payid show all</t>
+  </si>
+  <si>
+    <t>C002</t>
   </si>
 </sst>
 </file>
@@ -315,7 +376,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -629,7 +690,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -660,31 +721,31 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -712,7 +773,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -721,10 +782,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1052,19 +1113,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1125,7 +1186,7 @@
         <v>1000</v>
       </c>
       <c r="J2">
-        <v>10000</v>
+        <v>9000</v>
       </c>
       <c r="L2" s="40">
         <v>0.1</v>
@@ -1153,7 +1214,7 @@
       </c>
       <c r="J3">
         <f ca="1">IF(AND(B3="C001", C3&gt;0,E3=0),C3,IF(AND(B3="C001", H3 &gt; 0),J2-(I3+H3),J2-I3))</f>
-        <v>7500</v>
+        <v>6500</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -1178,7 +1239,7 @@
       </c>
       <c r="J4">
         <f ca="1">IF(AND(B4="C001", C4&gt;0,E4=0),C4,IF(AND(B4="C001", H4 &gt; 0),J3-(I4+H4),J3-I4))</f>
-        <v>5000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
@@ -1205,13 +1266,132 @@
         <v>4000</v>
       </c>
       <c r="J5">
-        <f ca="1">IF(AND(B5="C001", C5&gt;0,E5=0),C5,IF(AND(B5="C001", H5 &gt; 0),J4-(I5+H5),J4-I5))</f>
+        <f ca="1">J4-K5</f>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f ca="1">F5-H5</f>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="21">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="1">
+        <v>20000</v>
+      </c>
+      <c r="F8">
+        <v>2000</v>
+      </c>
+      <c r="I8">
+        <v>2000</v>
+      </c>
+      <c r="J8" s="1">
+        <f ca="1">C8-F8</f>
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="21">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="1">
+        <v>20000</v>
+      </c>
+      <c r="F9">
+        <v>3000</v>
+      </c>
+      <c r="J9" s="1">
+        <f ca="1">J8-F9</f>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="21">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="1">
+        <v>20000</v>
+      </c>
+      <c r="F10">
+        <v>5000</v>
+      </c>
+      <c r="J10" s="1">
+        <f ca="1">J9-F10</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="21">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="1">
+        <v>20000</v>
+      </c>
+      <c r="F11">
+        <v>10000</v>
+      </c>
+      <c r="H11">
+        <v>1000</v>
+      </c>
+      <c r="I11">
+        <f ca="1">F11-H11</f>
+        <v>9000</v>
+      </c>
+      <c r="J11" s="1">
+        <f ca="1">J10-F11</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>